<commit_message>
ultimo scrapy do 1 dia
</commit_message>
<xml_diff>
--- a/Planilha Apoio Pregao 90013_2024.xlsx
+++ b/Planilha Apoio Pregao 90013_2024.xlsx
@@ -45176,7 +45176,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AA1151"/>
+  <dimension ref="A1:AA1311"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -76368,6 +76368,4326 @@
       <c r="E1151" t="inlineStr">
         <is>
           <t>R$ 35,5200</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1151</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="D1152" t="inlineStr">
+        <is>
+          <t>R$ 36,8100</t>
+        </is>
+      </c>
+      <c r="E1152" t="inlineStr">
+        <is>
+          <t>R$ 36,8000</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1152</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>155</t>
+        </is>
+      </c>
+      <c r="D1153" t="inlineStr">
+        <is>
+          <t>R$ 27,5500</t>
+        </is>
+      </c>
+      <c r="E1153" t="inlineStr">
+        <is>
+          <t>R$ 27,5400</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1153</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="D1154" t="inlineStr">
+        <is>
+          <t>R$ 61,0200</t>
+        </is>
+      </c>
+      <c r="E1154" t="inlineStr">
+        <is>
+          <t>R$ 61,0100</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1154</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D1155" t="inlineStr">
+        <is>
+          <t>R$ 257,2100</t>
+        </is>
+      </c>
+      <c r="E1155" t="inlineStr">
+        <is>
+          <t>R$ 257,2000</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1155</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="D1156" t="inlineStr">
+        <is>
+          <t>R$ 96,4400</t>
+        </is>
+      </c>
+      <c r="E1156" t="inlineStr">
+        <is>
+          <t>R$ 96,4300</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1156</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="D1157" t="inlineStr">
+        <is>
+          <t>R$ 50,0500</t>
+        </is>
+      </c>
+      <c r="E1157" t="inlineStr">
+        <is>
+          <t>R$ 50,0400</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1157</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="D1158" t="inlineStr">
+        <is>
+          <t>R$ 65,5400</t>
+        </is>
+      </c>
+      <c r="E1158" t="inlineStr">
+        <is>
+          <t>R$ 65,5300</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1158</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="D1159" t="inlineStr">
+        <is>
+          <t>R$ 52,0700</t>
+        </is>
+      </c>
+      <c r="E1159" t="inlineStr">
+        <is>
+          <t>R$ 52,0600</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1159</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="D1160" t="inlineStr">
+        <is>
+          <t>R$ 137,9100</t>
+        </is>
+      </c>
+      <c r="E1160" t="inlineStr">
+        <is>
+          <t>R$ 137,9000</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1160</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D1161" t="inlineStr">
+        <is>
+          <t>R$ 133,8700</t>
+        </is>
+      </c>
+      <c r="E1161" t="inlineStr">
+        <is>
+          <t>R$ 133,8600</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1161</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="D1162" t="inlineStr">
+        <is>
+          <t>R$ 160,3100</t>
+        </is>
+      </c>
+      <c r="E1162" t="inlineStr">
+        <is>
+          <t>R$ 160,3000</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1162</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="D1163" t="inlineStr">
+        <is>
+          <t>R$ 71,5600</t>
+        </is>
+      </c>
+      <c r="E1163" t="inlineStr">
+        <is>
+          <t>R$ 71,5500</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1163</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="D1164" t="inlineStr">
+        <is>
+          <t>R$ 46,2400</t>
+        </is>
+      </c>
+      <c r="E1164" t="inlineStr">
+        <is>
+          <t>R$ 46,2300</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1164</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="D1165" t="inlineStr">
+        <is>
+          <t>R$ 47,7100</t>
+        </is>
+      </c>
+      <c r="E1165" t="inlineStr">
+        <is>
+          <t>R$ 47,7000</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1165</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D1166" t="inlineStr">
+        <is>
+          <t>R$ 63,6100</t>
+        </is>
+      </c>
+      <c r="E1166" t="inlineStr">
+        <is>
+          <t>R$ 63,6000</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1166</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="D1167" t="inlineStr">
+        <is>
+          <t>R$ 80,5400</t>
+        </is>
+      </c>
+      <c r="E1167" t="inlineStr">
+        <is>
+          <t>R$ 80,5300</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1167</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="D1168" t="inlineStr">
+        <is>
+          <t>R$ 9,4600</t>
+        </is>
+      </c>
+      <c r="E1168" t="inlineStr">
+        <is>
+          <t>R$ 9,4500</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1168</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D1169" t="inlineStr">
+        <is>
+          <t>R$ 6,9000</t>
+        </is>
+      </c>
+      <c r="E1169" t="inlineStr">
+        <is>
+          <t>R$ 6,8900</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1169</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>120</t>
+        </is>
+      </c>
+      <c r="D1170" t="inlineStr">
+        <is>
+          <t>R$ 9,5500</t>
+        </is>
+      </c>
+      <c r="E1170" t="inlineStr">
+        <is>
+          <t>R$ 9,5400</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1170</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>155</t>
+        </is>
+      </c>
+      <c r="D1171" t="inlineStr">
+        <is>
+          <t>R$ 3,6600</t>
+        </is>
+      </c>
+      <c r="E1171" t="inlineStr">
+        <is>
+          <t>R$ 3,6500</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1171</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="D1172" t="inlineStr">
+        <is>
+          <t>R$ 45,8900</t>
+        </is>
+      </c>
+      <c r="E1172" t="inlineStr">
+        <is>
+          <t>R$ 45,8800</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1172</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="D1173" t="inlineStr">
+        <is>
+          <t>R$ 30,6500</t>
+        </is>
+      </c>
+      <c r="E1173" t="inlineStr">
+        <is>
+          <t>R$ 30,6400</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1173</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>140</t>
+        </is>
+      </c>
+      <c r="D1174" t="inlineStr">
+        <is>
+          <t>R$ 57,1400</t>
+        </is>
+      </c>
+      <c r="E1174" t="inlineStr">
+        <is>
+          <t>R$ 57,1300</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1174</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="D1175" t="inlineStr">
+        <is>
+          <t>R$ 43,9600</t>
+        </is>
+      </c>
+      <c r="E1175" t="inlineStr">
+        <is>
+          <t>R$ 43,9500</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1175</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D1176" t="inlineStr">
+        <is>
+          <t>R$ 139,4100</t>
+        </is>
+      </c>
+      <c r="E1176" t="inlineStr">
+        <is>
+          <t>R$ 139,4000</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1176</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="D1177" t="inlineStr">
+        <is>
+          <t>R$ 6,0300</t>
+        </is>
+      </c>
+      <c r="E1177" t="inlineStr">
+        <is>
+          <t>R$ 6,0200</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1177</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D1178" t="inlineStr">
+        <is>
+          <t>R$ 1.739,6200</t>
+        </is>
+      </c>
+      <c r="E1178" t="inlineStr">
+        <is>
+          <t>R$ 1.739,6100</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1178</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D1179" t="inlineStr">
+        <is>
+          <t>R$ 1.409,3400</t>
+        </is>
+      </c>
+      <c r="E1179" t="inlineStr">
+        <is>
+          <t>R$ 1.409,3300</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1179</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="D1180" t="inlineStr">
+        <is>
+          <t>R$ 381,2900</t>
+        </is>
+      </c>
+      <c r="E1180" t="inlineStr">
+        <is>
+          <t>R$ 381,2800</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1180</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>1480</t>
+        </is>
+      </c>
+      <c r="D1181" t="inlineStr">
+        <is>
+          <t>R$ 7,9300</t>
+        </is>
+      </c>
+      <c r="E1181" t="inlineStr">
+        <is>
+          <t>R$ 7,9200</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1181</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>460</t>
+        </is>
+      </c>
+      <c r="D1182" t="inlineStr">
+        <is>
+          <t>R$ 3,9100</t>
+        </is>
+      </c>
+      <c r="E1182" t="inlineStr">
+        <is>
+          <t>R$ 3,9000</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1182</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D1183" t="inlineStr">
+        <is>
+          <t>R$ 3,9100</t>
+        </is>
+      </c>
+      <c r="E1183" t="inlineStr">
+        <is>
+          <t>R$ 3,9000</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1183</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>7470</t>
+        </is>
+      </c>
+      <c r="D1184" t="inlineStr">
+        <is>
+          <t>R$ 3,9100</t>
+        </is>
+      </c>
+      <c r="E1184" t="inlineStr">
+        <is>
+          <t>R$ 3,9000</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1184</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>2810</t>
+        </is>
+      </c>
+      <c r="D1185" t="inlineStr">
+        <is>
+          <t>R$ 3,9100</t>
+        </is>
+      </c>
+      <c r="E1185" t="inlineStr">
+        <is>
+          <t>R$ 3,9000</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1185</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>715</t>
+        </is>
+      </c>
+      <c r="D1186" t="inlineStr">
+        <is>
+          <t>R$ 3,9100</t>
+        </is>
+      </c>
+      <c r="E1186" t="inlineStr">
+        <is>
+          <t>R$ 3,9000</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1186</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>160</t>
+        </is>
+      </c>
+      <c r="D1187" t="inlineStr">
+        <is>
+          <t>R$ 31,4900</t>
+        </is>
+      </c>
+      <c r="E1187" t="inlineStr">
+        <is>
+          <t>R$ 31,4800</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1187</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>190</t>
+        </is>
+      </c>
+      <c r="D1188" t="inlineStr">
+        <is>
+          <t>R$ 2,6900</t>
+        </is>
+      </c>
+      <c r="E1188" t="inlineStr">
+        <is>
+          <t>R$ 2,6800</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1188</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>500</t>
+        </is>
+      </c>
+      <c r="D1189" t="inlineStr">
+        <is>
+          <t>R$ 3,9100</t>
+        </is>
+      </c>
+      <c r="E1189" t="inlineStr">
+        <is>
+          <t>R$ 3,9000</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1189</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="D1190" t="inlineStr">
+        <is>
+          <t>R$ 3,8500</t>
+        </is>
+      </c>
+      <c r="E1190" t="inlineStr">
+        <is>
+          <t>R$ 3,8400</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1190</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="D1191" t="inlineStr">
+        <is>
+          <t>R$ 3,8500</t>
+        </is>
+      </c>
+      <c r="E1191" t="inlineStr">
+        <is>
+          <t>R$ 3,8400</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1191</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>590</t>
+        </is>
+      </c>
+      <c r="D1192" t="inlineStr">
+        <is>
+          <t>R$ 3,9100</t>
+        </is>
+      </c>
+      <c r="E1192" t="inlineStr">
+        <is>
+          <t>R$ 3,9000</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1192</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>2300</t>
+        </is>
+      </c>
+      <c r="D1193" t="inlineStr">
+        <is>
+          <t>R$ 3,7800</t>
+        </is>
+      </c>
+      <c r="E1193" t="inlineStr">
+        <is>
+          <t>R$ 3,7700</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1193</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>580</t>
+        </is>
+      </c>
+      <c r="D1194" t="inlineStr">
+        <is>
+          <t>R$ 3,9100</t>
+        </is>
+      </c>
+      <c r="E1194" t="inlineStr">
+        <is>
+          <t>R$ 3,9000</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1194</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>85</t>
+        </is>
+      </c>
+      <c r="D1195" t="inlineStr">
+        <is>
+          <t>R$ 3,9100</t>
+        </is>
+      </c>
+      <c r="E1195" t="inlineStr">
+        <is>
+          <t>R$ 3,9000</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1195</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="D1196" t="inlineStr">
+        <is>
+          <t>R$ 6,2500</t>
+        </is>
+      </c>
+      <c r="E1196" t="inlineStr">
+        <is>
+          <t>R$ 6,2400</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1196</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>135</t>
+        </is>
+      </c>
+      <c r="D1197" t="inlineStr">
+        <is>
+          <t>R$ 7,6600</t>
+        </is>
+      </c>
+      <c r="E1197" t="inlineStr">
+        <is>
+          <t>R$ 7,6500</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1197</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>1260</t>
+        </is>
+      </c>
+      <c r="D1198" t="inlineStr">
+        <is>
+          <t>R$ 7,9700</t>
+        </is>
+      </c>
+      <c r="E1198" t="inlineStr">
+        <is>
+          <t>R$ 7,9600</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1198</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="D1199" t="inlineStr">
+        <is>
+          <t>R$ 16,5400</t>
+        </is>
+      </c>
+      <c r="E1199" t="inlineStr">
+        <is>
+          <t>R$ 16,5300</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1199</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="D1200" t="inlineStr">
+        <is>
+          <t>R$ 7,6600</t>
+        </is>
+      </c>
+      <c r="E1200" t="inlineStr">
+        <is>
+          <t>R$ 7,6500</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1200</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>535</t>
+        </is>
+      </c>
+      <c r="D1201" t="inlineStr">
+        <is>
+          <t>R$ 7,6600</t>
+        </is>
+      </c>
+      <c r="E1201" t="inlineStr">
+        <is>
+          <t>R$ 7,6500</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1201</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>1225</t>
+        </is>
+      </c>
+      <c r="D1202" t="inlineStr">
+        <is>
+          <t>R$ 10,6400</t>
+        </is>
+      </c>
+      <c r="E1202" t="inlineStr">
+        <is>
+          <t>R$ 10,6300</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1202</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>1475</t>
+        </is>
+      </c>
+      <c r="D1203" t="inlineStr">
+        <is>
+          <t>R$ 7,8200</t>
+        </is>
+      </c>
+      <c r="E1203" t="inlineStr">
+        <is>
+          <t>R$ 7,8100</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1203</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>90</t>
+        </is>
+      </c>
+      <c r="D1204" t="inlineStr">
+        <is>
+          <t>R$ 7,8200</t>
+        </is>
+      </c>
+      <c r="E1204" t="inlineStr">
+        <is>
+          <t>R$ 7,8100</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1204</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="D1205" t="inlineStr">
+        <is>
+          <t>R$ 7,8200</t>
+        </is>
+      </c>
+      <c r="E1205" t="inlineStr">
+        <is>
+          <t>R$ 7,8100</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1205</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>195</t>
+        </is>
+      </c>
+      <c r="D1206" t="inlineStr">
+        <is>
+          <t>R$ 39,2400</t>
+        </is>
+      </c>
+      <c r="E1206" t="inlineStr">
+        <is>
+          <t>R$ 39,2300</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1206</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>1710</t>
+        </is>
+      </c>
+      <c r="D1207" t="inlineStr">
+        <is>
+          <t>R$ 8,1600</t>
+        </is>
+      </c>
+      <c r="E1207" t="inlineStr">
+        <is>
+          <t>R$ 8,1500</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1207</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D1208" t="inlineStr">
+        <is>
+          <t>R$ 18,6300</t>
+        </is>
+      </c>
+      <c r="E1208" t="inlineStr">
+        <is>
+          <t>R$ 18,6200</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1208</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="D1209" t="inlineStr">
+        <is>
+          <t>R$ 23,4700</t>
+        </is>
+      </c>
+      <c r="E1209" t="inlineStr">
+        <is>
+          <t>R$ 23,4600</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1209</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>115</t>
+        </is>
+      </c>
+      <c r="D1210" t="inlineStr">
+        <is>
+          <t>R$ 7,5000</t>
+        </is>
+      </c>
+      <c r="E1210" t="inlineStr">
+        <is>
+          <t>R$ 7,4900</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1210</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>145</t>
+        </is>
+      </c>
+      <c r="D1211" t="inlineStr">
+        <is>
+          <t>R$ 0,9000</t>
+        </is>
+      </c>
+      <c r="E1211" t="inlineStr">
+        <is>
+          <t>R$ 0,8900</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1211</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="D1212" t="inlineStr">
+        <is>
+          <t>R$ 7,8200</t>
+        </is>
+      </c>
+      <c r="E1212" t="inlineStr">
+        <is>
+          <t>R$ 7,8100</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1212</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="D1213" t="inlineStr">
+        <is>
+          <t>R$ 7,8200</t>
+        </is>
+      </c>
+      <c r="E1213" t="inlineStr">
+        <is>
+          <t>R$ 7,8100</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1213</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="D1214" t="inlineStr">
+        <is>
+          <t>R$ 7,8200</t>
+        </is>
+      </c>
+      <c r="E1214" t="inlineStr">
+        <is>
+          <t>R$ 7,8100</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1214</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>665</t>
+        </is>
+      </c>
+      <c r="D1215" t="inlineStr">
+        <is>
+          <t>R$ 13,1000</t>
+        </is>
+      </c>
+      <c r="E1215" t="inlineStr">
+        <is>
+          <t>R$ 13,0900</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1215</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="D1216" t="inlineStr">
+        <is>
+          <t>R$ 7,8200</t>
+        </is>
+      </c>
+      <c r="E1216" t="inlineStr">
+        <is>
+          <t>R$ 7,8100</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1216</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="D1217" t="inlineStr">
+        <is>
+          <t>R$ 7,8200</t>
+        </is>
+      </c>
+      <c r="E1217" t="inlineStr">
+        <is>
+          <t>R$ 7,8100</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1217</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="D1218" t="inlineStr">
+        <is>
+          <t>R$ 3,7800</t>
+        </is>
+      </c>
+      <c r="E1218" t="inlineStr">
+        <is>
+          <t>R$ 3,7700</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1218</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>1540</t>
+        </is>
+      </c>
+      <c r="D1219" t="inlineStr">
+        <is>
+          <t>R$ 7,8200</t>
+        </is>
+      </c>
+      <c r="E1219" t="inlineStr">
+        <is>
+          <t>R$ 7,8100</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1219</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>110</t>
+        </is>
+      </c>
+      <c r="D1220" t="inlineStr">
+        <is>
+          <t>R$ 40,4000</t>
+        </is>
+      </c>
+      <c r="E1220" t="inlineStr">
+        <is>
+          <t>R$ 40,3900</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1220</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="D1221" t="inlineStr">
+        <is>
+          <t>R$ 35,2700</t>
+        </is>
+      </c>
+      <c r="E1221" t="inlineStr">
+        <is>
+          <t>R$ 35,2600</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1221</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>255</t>
+        </is>
+      </c>
+      <c r="D1222" t="inlineStr">
+        <is>
+          <t>R$ 7,8200</t>
+        </is>
+      </c>
+      <c r="E1222" t="inlineStr">
+        <is>
+          <t>R$ 7,8100</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1222</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D1223" t="inlineStr">
+        <is>
+          <t>R$ 7,6600</t>
+        </is>
+      </c>
+      <c r="E1223" t="inlineStr">
+        <is>
+          <t>R$ 7,6500</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1223</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>185</t>
+        </is>
+      </c>
+      <c r="D1224" t="inlineStr">
+        <is>
+          <t>R$ 7,8200</t>
+        </is>
+      </c>
+      <c r="E1224" t="inlineStr">
+        <is>
+          <t>R$ 7,8100</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1224</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>115</t>
+        </is>
+      </c>
+      <c r="D1225" t="inlineStr">
+        <is>
+          <t>R$ 7,8900</t>
+        </is>
+      </c>
+      <c r="E1225" t="inlineStr">
+        <is>
+          <t>R$ 7,8800</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1225</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>1025</t>
+        </is>
+      </c>
+      <c r="D1226" t="inlineStr">
+        <is>
+          <t>R$ 4,5300</t>
+        </is>
+      </c>
+      <c r="E1226" t="inlineStr">
+        <is>
+          <t>R$ 4,5200</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1226</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="D1227" t="inlineStr">
+        <is>
+          <t>R$ 6,2500</t>
+        </is>
+      </c>
+      <c r="E1227" t="inlineStr">
+        <is>
+          <t>R$ 6,2400</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1227</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>85</t>
+        </is>
+      </c>
+      <c r="D1228" t="inlineStr">
+        <is>
+          <t>R$ 9,4000</t>
+        </is>
+      </c>
+      <c r="E1228" t="inlineStr">
+        <is>
+          <t>R$ 9,3900</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1228</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>690</t>
+        </is>
+      </c>
+      <c r="D1229" t="inlineStr">
+        <is>
+          <t>R$ 6,2500</t>
+        </is>
+      </c>
+      <c r="E1229" t="inlineStr">
+        <is>
+          <t>R$ 6,2400</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1229</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>380</t>
+        </is>
+      </c>
+      <c r="D1230" t="inlineStr">
+        <is>
+          <t>R$ 6,1300</t>
+        </is>
+      </c>
+      <c r="E1230" t="inlineStr">
+        <is>
+          <t>R$ 6,1200</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1230</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>85</t>
+        </is>
+      </c>
+      <c r="D1231" t="inlineStr">
+        <is>
+          <t>R$ 6,0300</t>
+        </is>
+      </c>
+      <c r="E1231" t="inlineStr">
+        <is>
+          <t>R$ 6,0200</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1231</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="D1232" t="inlineStr">
+        <is>
+          <t>R$ 9,4000</t>
+        </is>
+      </c>
+      <c r="E1232" t="inlineStr">
+        <is>
+          <t>R$ 9,3900</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1232</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>585</t>
+        </is>
+      </c>
+      <c r="D1233" t="inlineStr">
+        <is>
+          <t>R$ 6,0300</t>
+        </is>
+      </c>
+      <c r="E1233" t="inlineStr">
+        <is>
+          <t>R$ 6,0200</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1233</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>4405</t>
+        </is>
+      </c>
+      <c r="D1234" t="inlineStr">
+        <is>
+          <t>R$ 3,5900</t>
+        </is>
+      </c>
+      <c r="E1234" t="inlineStr">
+        <is>
+          <t>R$ 3,5800</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1234</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="D1235" t="inlineStr">
+        <is>
+          <t>R$ 9,3600</t>
+        </is>
+      </c>
+      <c r="E1235" t="inlineStr">
+        <is>
+          <t>R$ 9,3500</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1235</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>155</t>
+        </is>
+      </c>
+      <c r="D1236" t="inlineStr">
+        <is>
+          <t>R$ 9,1700</t>
+        </is>
+      </c>
+      <c r="E1236" t="inlineStr">
+        <is>
+          <t>R$ 9,1600</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1236</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>270</t>
+        </is>
+      </c>
+      <c r="D1237" t="inlineStr">
+        <is>
+          <t>R$ 9,4000</t>
+        </is>
+      </c>
+      <c r="E1237" t="inlineStr">
+        <is>
+          <t>R$ 9,3900</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1237</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>705</t>
+        </is>
+      </c>
+      <c r="D1238" t="inlineStr">
+        <is>
+          <t>R$ 9,3600</t>
+        </is>
+      </c>
+      <c r="E1238" t="inlineStr">
+        <is>
+          <t>R$ 9,3500</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1238</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>290</t>
+        </is>
+      </c>
+      <c r="D1239" t="inlineStr">
+        <is>
+          <t>R$ 9,2800</t>
+        </is>
+      </c>
+      <c r="E1239" t="inlineStr">
+        <is>
+          <t>R$ 9,2700</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1239</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>535</t>
+        </is>
+      </c>
+      <c r="D1240" t="inlineStr">
+        <is>
+          <t>R$ 9,3600</t>
+        </is>
+      </c>
+      <c r="E1240" t="inlineStr">
+        <is>
+          <t>R$ 9,3500</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1240</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="D1241" t="inlineStr">
+        <is>
+          <t>R$ 9,3600</t>
+        </is>
+      </c>
+      <c r="E1241" t="inlineStr">
+        <is>
+          <t>R$ 9,3500</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1241</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="D1242" t="inlineStr">
+        <is>
+          <t>R$ 9,3600</t>
+        </is>
+      </c>
+      <c r="E1242" t="inlineStr">
+        <is>
+          <t>R$ 9,3500</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1242</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="D1243" t="inlineStr">
+        <is>
+          <t>R$ 9,4000</t>
+        </is>
+      </c>
+      <c r="E1243" t="inlineStr">
+        <is>
+          <t>R$ 9,3900</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1243</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="D1244" t="inlineStr">
+        <is>
+          <t>R$ 75,9900</t>
+        </is>
+      </c>
+      <c r="E1244" t="inlineStr">
+        <is>
+          <t>R$ 75,9800</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1244</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="D1245" t="inlineStr">
+        <is>
+          <t>R$ 295,8100</t>
+        </is>
+      </c>
+      <c r="E1245" t="inlineStr">
+        <is>
+          <t>R$ 295,8000</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1245</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>160</t>
+        </is>
+      </c>
+      <c r="D1246" t="inlineStr">
+        <is>
+          <t>R$ 42,7700</t>
+        </is>
+      </c>
+      <c r="E1246" t="inlineStr">
+        <is>
+          <t>R$ 42,7600</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1246</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>445</t>
+        </is>
+      </c>
+      <c r="D1247" t="inlineStr">
+        <is>
+          <t>R$ 32,8000</t>
+        </is>
+      </c>
+      <c r="E1247" t="inlineStr">
+        <is>
+          <t>R$ 32,7900</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1247</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="D1248" t="inlineStr">
+        <is>
+          <t>R$ 49,8300</t>
+        </is>
+      </c>
+      <c r="E1248" t="inlineStr">
+        <is>
+          <t>R$ 49,8200</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1248</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>85</t>
+        </is>
+      </c>
+      <c r="D1249" t="inlineStr">
+        <is>
+          <t>R$ 40,2700</t>
+        </is>
+      </c>
+      <c r="E1249" t="inlineStr">
+        <is>
+          <t>R$ 40,2600</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1249</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>705</t>
+        </is>
+      </c>
+      <c r="D1250" t="inlineStr">
+        <is>
+          <t>R$ 45,7500</t>
+        </is>
+      </c>
+      <c r="E1250" t="inlineStr">
+        <is>
+          <t>R$ 45,7400</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1250</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="D1251" t="inlineStr">
+        <is>
+          <t>R$ 207,5400</t>
+        </is>
+      </c>
+      <c r="E1251" t="inlineStr">
+        <is>
+          <t>R$ 207,5300</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1251</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="D1252" t="inlineStr">
+        <is>
+          <t>R$ 19,2400</t>
+        </is>
+      </c>
+      <c r="E1252" t="inlineStr">
+        <is>
+          <t>R$ 19,2300</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1252</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D1253" t="inlineStr">
+        <is>
+          <t>R$ 14,7200</t>
+        </is>
+      </c>
+      <c r="E1253" t="inlineStr">
+        <is>
+          <t>R$ 14,7100</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1253</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="D1254" t="inlineStr">
+        <is>
+          <t>R$ 20,5000</t>
+        </is>
+      </c>
+      <c r="E1254" t="inlineStr">
+        <is>
+          <t>R$ 20,4900</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1254</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="D1255" t="inlineStr">
+        <is>
+          <t>R$ 46,3800</t>
+        </is>
+      </c>
+      <c r="E1255" t="inlineStr">
+        <is>
+          <t>R$ 46,3700</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1255</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>440</t>
+        </is>
+      </c>
+      <c r="D1256" t="inlineStr">
+        <is>
+          <t>R$ 86,9900</t>
+        </is>
+      </c>
+      <c r="E1256" t="inlineStr">
+        <is>
+          <t>R$ 86,9800</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1256</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="D1257" t="inlineStr">
+        <is>
+          <t>R$ 860,5600</t>
+        </is>
+      </c>
+      <c r="E1257" t="inlineStr">
+        <is>
+          <t>R$ 860,5500</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1257</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="D1258" t="inlineStr">
+        <is>
+          <t>R$ 901,5500</t>
+        </is>
+      </c>
+      <c r="E1258" t="inlineStr">
+        <is>
+          <t>R$ 901,5400</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1258</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D1259" t="inlineStr">
+        <is>
+          <t>R$ 754,2800</t>
+        </is>
+      </c>
+      <c r="E1259" t="inlineStr">
+        <is>
+          <t>R$ 754,2700</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1259</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="D1260" t="inlineStr">
+        <is>
+          <t>R$ 790,8600</t>
+        </is>
+      </c>
+      <c r="E1260" t="inlineStr">
+        <is>
+          <t>R$ 790,8500</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1260</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>380</t>
+        </is>
+      </c>
+      <c r="D1261" t="inlineStr">
+        <is>
+          <t>R$ 1,7300</t>
+        </is>
+      </c>
+      <c r="E1261" t="inlineStr">
+        <is>
+          <t>R$ 1,7200</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1261</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>945</t>
+        </is>
+      </c>
+      <c r="D1262" t="inlineStr">
+        <is>
+          <t>R$ 46,3400</t>
+        </is>
+      </c>
+      <c r="E1262" t="inlineStr">
+        <is>
+          <t>R$ 46,3300</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1262</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="D1263" t="inlineStr">
+        <is>
+          <t>R$ 111,4800</t>
+        </is>
+      </c>
+      <c r="E1263" t="inlineStr">
+        <is>
+          <t>R$ 111,4700</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1263</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="D1264" t="inlineStr">
+        <is>
+          <t>R$ 56,9700</t>
+        </is>
+      </c>
+      <c r="E1264" t="inlineStr">
+        <is>
+          <t>R$ 56,9600</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1264</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D1265" t="inlineStr">
+        <is>
+          <t>R$ 8,4600</t>
+        </is>
+      </c>
+      <c r="E1265" t="inlineStr">
+        <is>
+          <t>R$ 8,4500</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1265</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="D1266" t="inlineStr">
+        <is>
+          <t>R$ 161,7600</t>
+        </is>
+      </c>
+      <c r="E1266" t="inlineStr">
+        <is>
+          <t>R$ 161,7500</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1266</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D1267" t="inlineStr">
+        <is>
+          <t>R$ 181,1600</t>
+        </is>
+      </c>
+      <c r="E1267" t="inlineStr">
+        <is>
+          <t>R$ 181,1500</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1267</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="D1268" t="inlineStr">
+        <is>
+          <t>R$ 171,8600</t>
+        </is>
+      </c>
+      <c r="E1268" t="inlineStr">
+        <is>
+          <t>R$ 171,8500</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1268</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="D1269" t="inlineStr">
+        <is>
+          <t>R$ 111,8400</t>
+        </is>
+      </c>
+      <c r="E1269" t="inlineStr">
+        <is>
+          <t>R$ 111,8300</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1269</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D1270" t="inlineStr">
+        <is>
+          <t>R$ 105,0400</t>
+        </is>
+      </c>
+      <c r="E1270" t="inlineStr">
+        <is>
+          <t>R$ 105,0300</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1270</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D1271" t="inlineStr">
+        <is>
+          <t>R$ 171,4900</t>
+        </is>
+      </c>
+      <c r="E1271" t="inlineStr">
+        <is>
+          <t>R$ 171,4800</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1271</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D1272" t="inlineStr">
+        <is>
+          <t>R$ 60,9200</t>
+        </is>
+      </c>
+      <c r="E1272" t="inlineStr">
+        <is>
+          <t>R$ 60,9100</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1272</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+      <c r="D1273" t="inlineStr">
+        <is>
+          <t>R$ 59,6400</t>
+        </is>
+      </c>
+      <c r="E1273" t="inlineStr">
+        <is>
+          <t>R$ 59,6300</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1273</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>460</t>
+        </is>
+      </c>
+      <c r="D1274" t="inlineStr">
+        <is>
+          <t>R$ 9,4000</t>
+        </is>
+      </c>
+      <c r="E1274" t="inlineStr">
+        <is>
+          <t>R$ 9,3900</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1274</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>115</t>
+        </is>
+      </c>
+      <c r="D1275" t="inlineStr">
+        <is>
+          <t>R$ 56,4900</t>
+        </is>
+      </c>
+      <c r="E1275" t="inlineStr">
+        <is>
+          <t>R$ 56,4800</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1275</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>730</t>
+        </is>
+      </c>
+      <c r="D1276" t="inlineStr">
+        <is>
+          <t>R$ 9,4000</t>
+        </is>
+      </c>
+      <c r="E1276" t="inlineStr">
+        <is>
+          <t>R$ 9,3900</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1276</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="D1277" t="inlineStr">
+        <is>
+          <t>R$ 9,4000</t>
+        </is>
+      </c>
+      <c r="E1277" t="inlineStr">
+        <is>
+          <t>R$ 9,3900</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1277</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>805</t>
+        </is>
+      </c>
+      <c r="D1278" t="inlineStr">
+        <is>
+          <t>R$ 9,4000</t>
+        </is>
+      </c>
+      <c r="E1278" t="inlineStr">
+        <is>
+          <t>R$ 9,3900</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1278</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>560</t>
+        </is>
+      </c>
+      <c r="D1279" t="inlineStr">
+        <is>
+          <t>R$ 9,4000</t>
+        </is>
+      </c>
+      <c r="E1279" t="inlineStr">
+        <is>
+          <t>R$ 9,3900</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1279</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>2075</t>
+        </is>
+      </c>
+      <c r="D1280" t="inlineStr">
+        <is>
+          <t>R$ 9,3600</t>
+        </is>
+      </c>
+      <c r="E1280" t="inlineStr">
+        <is>
+          <t>R$ 9,3500</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1280</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>420</t>
+        </is>
+      </c>
+      <c r="D1281" t="inlineStr">
+        <is>
+          <t>R$ 166,0200</t>
+        </is>
+      </c>
+      <c r="E1281" t="inlineStr">
+        <is>
+          <t>R$ 166,0100</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1281</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>1385</t>
+        </is>
+      </c>
+      <c r="D1282" t="inlineStr">
+        <is>
+          <t>R$ 9,3600</t>
+        </is>
+      </c>
+      <c r="E1282" t="inlineStr">
+        <is>
+          <t>R$ 9,3500</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1282</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>665</t>
+        </is>
+      </c>
+      <c r="D1283" t="inlineStr">
+        <is>
+          <t>R$ 9,3800</t>
+        </is>
+      </c>
+      <c r="E1283" t="inlineStr">
+        <is>
+          <t>R$ 9,3700</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1283</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="D1284" t="inlineStr">
+        <is>
+          <t>R$ 9,3600</t>
+        </is>
+      </c>
+      <c r="E1284" t="inlineStr">
+        <is>
+          <t>R$ 9,3500</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1284</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>565</t>
+        </is>
+      </c>
+      <c r="D1285" t="inlineStr">
+        <is>
+          <t>R$ 9,1700</t>
+        </is>
+      </c>
+      <c r="E1285" t="inlineStr">
+        <is>
+          <t>R$ 9,1600</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1285</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="D1286" t="inlineStr">
+        <is>
+          <t>R$ 9,3600</t>
+        </is>
+      </c>
+      <c r="E1286" t="inlineStr">
+        <is>
+          <t>R$ 9,3500</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1286</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>4065</t>
+        </is>
+      </c>
+      <c r="D1287" t="inlineStr">
+        <is>
+          <t>R$ 9,3600</t>
+        </is>
+      </c>
+      <c r="E1287" t="inlineStr">
+        <is>
+          <t>R$ 9,3500</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1287</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>3580</t>
+        </is>
+      </c>
+      <c r="D1288" t="inlineStr">
+        <is>
+          <t>R$ 9,1700</t>
+        </is>
+      </c>
+      <c r="E1288" t="inlineStr">
+        <is>
+          <t>R$ 9,1600</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1288</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>405</t>
+        </is>
+      </c>
+      <c r="D1289" t="inlineStr">
+        <is>
+          <t>R$ 9,3600</t>
+        </is>
+      </c>
+      <c r="E1289" t="inlineStr">
+        <is>
+          <t>R$ 9,3500</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1289</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>105</t>
+        </is>
+      </c>
+      <c r="D1290" t="inlineStr">
+        <is>
+          <t>R$ 9,1700</t>
+        </is>
+      </c>
+      <c r="E1290" t="inlineStr">
+        <is>
+          <t>R$ 9,1600</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1290</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>155</t>
+        </is>
+      </c>
+      <c r="D1291" t="inlineStr">
+        <is>
+          <t>R$ 9,4000</t>
+        </is>
+      </c>
+      <c r="E1291" t="inlineStr">
+        <is>
+          <t>R$ 9,3900</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1291</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>155</t>
+        </is>
+      </c>
+      <c r="D1292" t="inlineStr">
+        <is>
+          <t>R$ 9,3600</t>
+        </is>
+      </c>
+      <c r="E1292" t="inlineStr">
+        <is>
+          <t>R$ 9,3500</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1292</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="D1293" t="inlineStr">
+        <is>
+          <t>R$ 9,4000</t>
+        </is>
+      </c>
+      <c r="E1293" t="inlineStr">
+        <is>
+          <t>R$ 9,3900</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1293</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>650</t>
+        </is>
+      </c>
+      <c r="D1294" t="inlineStr">
+        <is>
+          <t>R$ 9,1700</t>
+        </is>
+      </c>
+      <c r="E1294" t="inlineStr">
+        <is>
+          <t>R$ 9,1600</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1294</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>125</t>
+        </is>
+      </c>
+      <c r="D1295" t="inlineStr">
+        <is>
+          <t>R$ 9,4000</t>
+        </is>
+      </c>
+      <c r="E1295" t="inlineStr">
+        <is>
+          <t>R$ 9,3900</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1295</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D1296" t="inlineStr">
+        <is>
+          <t>R$ 11,7300</t>
+        </is>
+      </c>
+      <c r="E1296" t="inlineStr">
+        <is>
+          <t>R$ 11,7200</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1296</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>75</t>
+        </is>
+      </c>
+      <c r="D1297" t="inlineStr">
+        <is>
+          <t>R$ 97,7300</t>
+        </is>
+      </c>
+      <c r="E1297" t="inlineStr">
+        <is>
+          <t>R$ 97,7200</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1297</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>195</t>
+        </is>
+      </c>
+      <c r="D1298" t="inlineStr">
+        <is>
+          <t>R$ 1.328,8700</t>
+        </is>
+      </c>
+      <c r="E1298" t="inlineStr">
+        <is>
+          <t>R$ 1.328,8600</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1298</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="D1299" t="inlineStr">
+        <is>
+          <t>R$ 1.640,9100</t>
+        </is>
+      </c>
+      <c r="E1299" t="inlineStr">
+        <is>
+          <t>R$ 1.640,9000</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1299</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D1300" t="inlineStr">
+        <is>
+          <t>R$ 1.206,1000</t>
+        </is>
+      </c>
+      <c r="E1300" t="inlineStr">
+        <is>
+          <t>R$ 1.206,0900</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1300</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="D1301" t="inlineStr">
+        <is>
+          <t>R$ 1.375,4800</t>
+        </is>
+      </c>
+      <c r="E1301" t="inlineStr">
+        <is>
+          <t>R$ 1.375,4700</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1301</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>85</t>
+        </is>
+      </c>
+      <c r="D1302" t="inlineStr">
+        <is>
+          <t>R$ 1.014,3900</t>
+        </is>
+      </c>
+      <c r="E1302" t="inlineStr">
+        <is>
+          <t>R$ 1.014,3800</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1302</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="D1303" t="inlineStr">
+        <is>
+          <t>R$ 1.038,0300</t>
+        </is>
+      </c>
+      <c r="E1303" t="inlineStr">
+        <is>
+          <t>R$ 1.038,0200</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1303</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="D1304" t="inlineStr">
+        <is>
+          <t>R$ 1.615,6900</t>
+        </is>
+      </c>
+      <c r="E1304" t="inlineStr">
+        <is>
+          <t>R$ 1.615,6800</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1304</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D1305" t="inlineStr">
+        <is>
+          <t>R$ 144,9300</t>
+        </is>
+      </c>
+      <c r="E1305" t="inlineStr">
+        <is>
+          <t>R$ 144,9200</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1305</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D1306" t="inlineStr">
+        <is>
+          <t>R$ 3.512,9000</t>
+        </is>
+      </c>
+      <c r="E1306" t="inlineStr">
+        <is>
+          <t>R$ 3.512,8900</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1306</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="D1307" t="inlineStr">
+        <is>
+          <t>R$ 356,6000</t>
+        </is>
+      </c>
+      <c r="E1307" t="inlineStr">
+        <is>
+          <t>R$ 356,5900</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1307</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>795</t>
+        </is>
+      </c>
+      <c r="D1308" t="inlineStr">
+        <is>
+          <t>R$ 34,0900</t>
+        </is>
+      </c>
+      <c r="E1308" t="inlineStr">
+        <is>
+          <t>R$ 34,0800</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1308</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="D1309" t="inlineStr">
+        <is>
+          <t>R$ 228,0900</t>
+        </is>
+      </c>
+      <c r="E1309" t="inlineStr">
+        <is>
+          <t>R$ 228,0800</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1309</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>595</t>
+        </is>
+      </c>
+      <c r="D1310" t="inlineStr">
+        <is>
+          <t>R$ 267,4400</t>
+        </is>
+      </c>
+      <c r="E1310" t="inlineStr">
+        <is>
+          <t>R$ 267,4300</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1310</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>H8 ALS INDUSTRIA AERONAUTICA LTDA</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="D1311" t="inlineStr">
+        <is>
+          <t>R$ 301,1000</t>
+        </is>
+      </c>
+      <c r="E1311" t="inlineStr">
+        <is>
+          <t>R$ 301,0900</t>
         </is>
       </c>
     </row>

</xml_diff>